<commit_message>
a bunch of work for revisions
</commit_message>
<xml_diff>
--- a/tables/TableS1_stock_selection.xlsx
+++ b/tables/TableS1_stock_selection.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cfree/Dropbox/Chris/Rutgers/projects/forage_fish/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60C1074D-09A8-DA42-923B-934CF56AA31C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6B14C34-8E46-3F49-B4D2-E52379806638}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31640" yWindow="2660" windowWidth="23040" windowHeight="15000" activeTab="3" xr2:uid="{0AE76B40-AA2F-1B4E-B4AD-5ADE4AE9F06F}"/>
+    <workbookView xWindow="28160" yWindow="2660" windowWidth="23040" windowHeight="15000" xr2:uid="{0AE76B40-AA2F-1B4E-B4AD-5ADE4AE9F06F}"/>
   </bookViews>
   <sheets>
     <sheet name="All" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="29">
   <si>
     <t>Criteria</t>
   </si>
@@ -90,9 +90,6 @@
     <t>Populations with ≥15 years of data</t>
   </si>
   <si>
-    <t>Removed 2 population w/ wild dynamics</t>
-  </si>
-  <si>
     <t>Populations in 4 study regions</t>
   </si>
   <si>
@@ -117,7 +114,7 @@
     <t>Removed 3 highly correlated Peruvian bird populations</t>
   </si>
   <si>
-    <t>Removed 2 population with wild dynamics</t>
+    <t>Removed 2 populations preventing model convergence because they exhibited population dynamics wildly divergent from stationary logistic population growth</t>
   </si>
 </sst>
 </file>
@@ -513,8 +510,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD2D7E20-AD63-4A44-94FC-6D39DABC98C7}">
   <dimension ref="A2:C31"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -537,7 +534,7 @@
     </row>
     <row r="3" spans="1:3" ht="18" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
@@ -560,7 +557,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B6">
         <v>54</v>
@@ -579,7 +576,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B8">
         <v>47</v>
@@ -601,7 +598,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -622,7 +619,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B14">
         <v>147</v>
@@ -678,7 +675,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
@@ -718,7 +715,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B27" s="3">
         <v>23</v>
@@ -726,7 +723,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B28" s="3">
         <v>20</v>
@@ -734,7 +731,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B29" s="3">
         <v>18</v>
@@ -745,7 +742,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -798,7 +795,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B5">
         <v>54</v>
@@ -817,7 +814,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B7">
         <v>47</v>
@@ -882,7 +879,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B5">
         <v>147</v>
@@ -950,8 +947,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8E95CBC-6C6F-0343-9187-DD99D750F6A5}">
   <dimension ref="A2:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1009,7 +1006,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B7" s="3">
         <v>23</v>
@@ -1017,7 +1014,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B8" s="3">
         <v>20</v>
@@ -1025,7 +1022,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="B9" s="3">
         <v>18</v>

</xml_diff>